<commit_message>
competencias e habilidades do ensino medio adicionadas
</commit_message>
<xml_diff>
--- a/ensino_medio/habilidades_ch_em.xlsx
+++ b/ensino_medio/habilidades_ch_em.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\aplicacao_bncc\ensino_medio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A92DEBF0-7D0C-425D-B3A2-1D042E4B7734}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D5AEBFC-1C0D-4BAD-8CF1-3AF829FE2853}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{843C204E-0D25-4DA0-8C07-4E2429C3F3BB}"/>
   </bookViews>
@@ -33,9 +33,6 @@
     <t>cod_hab</t>
   </si>
   <si>
-    <t>habilidades_ch_em</t>
-  </si>
-  <si>
     <t>1º, 2º, 3º</t>
   </si>
   <si>
@@ -517,13 +514,16 @@
       </rPr>
       <t>Analisar e experimentar diversos processos de remidiação de produções multissemióticas, multimídia e transmídia, desenvolvendo diferentes modos de participação e intervenção social.</t>
     </r>
+  </si>
+  <si>
+    <t>habilidades</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,6 +536,14 @@
       <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -585,7 +593,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -596,6 +604,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -910,15 +919,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5037C29B-C0C4-41B8-98D3-8FE82599E6AB}">
-  <dimension ref="A1:C33"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -926,362 +935,364 @@
         <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="4"/>
+    </row>
+    <row r="3" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="3" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="3" t="s">
+    </row>
+    <row r="5" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="3" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="3" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="3" t="s">
+    </row>
+    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="3" t="s">
+    </row>
+    <row r="9" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="3" t="s">
+    </row>
+    <row r="11" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="3" t="s">
+    </row>
+    <row r="12" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="12" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="3" t="s">
+    </row>
+    <row r="13" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="3" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B14" s="2" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="14" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="3" t="s">
+    </row>
+    <row r="15" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="15" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B15" s="2" t="s">
+      <c r="C15" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C15" s="3" t="s">
+    </row>
+    <row r="16" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="16" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B16" s="2" t="s">
+      <c r="C16" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>34</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>36</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="C19" s="3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B20" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>40</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="390" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B21" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C23" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="C23" s="3" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C24" s="3" t="s">
         <v>48</v>
-      </c>
-      <c r="C24" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B25" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B26" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>54</v>
-      </c>
-      <c r="C27" s="3" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>56</v>
-      </c>
-      <c r="C28" s="3" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B29" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>58</v>
-      </c>
-      <c r="C29" s="3" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B30" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="C30" s="3" t="s">
         <v>60</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B31" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C31" s="3" t="s">
         <v>62</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B32" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C32" s="3" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" s="3" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>